<commit_message>
blancoRestGenerator now starting! Separate telegram and telegramProcess generator from old blancoRest. Now, blancoRest will obsoleted in near future.
</commit_message>
<xml_diff>
--- a/meta/objects/ApiDeleteTelegram.xlsx
+++ b/meta/objects/ApiDeleteTelegram.xlsx
@@ -1,30 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRest/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FDC53D-686A-1F4E-B675-F41759DF323A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1880" windowWidth="24320" windowHeight="14120" tabRatio="640"/>
+    <workbookView xWindow="3940" yWindow="2260" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
+    <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="accessScope">config!$B$4:$B$6</definedName>
+    <definedName name="accessScope2">config!$B$4:$B$5</definedName>
+    <definedName name="adjustDefaultValue">config!$J$4:$J$5</definedName>
+    <definedName name="adjustFiledName">config!$H$4:$H$5</definedName>
+    <definedName name="createToString">config!$F$4:$F$5</definedName>
+    <definedName name="isAbstract">config!$D$4:$D$5</definedName>
+    <definedName name="Submit有無" localSheetId="1">#REF!</definedName>
     <definedName name="Submit有無">#REF!</definedName>
+    <definedName name="toString">config!$F$4:$F$5</definedName>
+    <definedName name="Validate実装パターン" localSheetId="1">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
+    <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
+    <definedName name="デリミタ" localSheetId="1">#REF!</definedName>
     <definedName name="デリミタ">#REF!</definedName>
+    <definedName name="デリミタ選択肢" localSheetId="1">#REF!</definedName>
     <definedName name="デリミタ選択肢">#REF!</definedName>
+    <definedName name="型" localSheetId="1">#REF!</definedName>
     <definedName name="型">#REF!</definedName>
+    <definedName name="項目型" localSheetId="1">#REF!</definedName>
     <definedName name="項目型">#REF!</definedName>
+    <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>クラス名</t>
   </si>
@@ -142,12 +162,96 @@
     <t>\blanco\rest\valueobject</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>バリューオブジェクト定義書 設定シート</t>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>様式 ver 0.9.9 (2007.12.06)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アクセス</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>抽象クラス</t>
+    <rPh sb="0" eb="2">
+      <t>チュウショウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>toStringメソッド</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>フィールド名の変形</t>
+    <rPh sb="5" eb="6">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヘンケイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>デフォルト値の変形</t>
+    <rPh sb="7" eb="9">
+      <t>ヘンケイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>public</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>toStringメソッドの生成</t>
+    <rPh sb="13" eb="15">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>フィールド名の変形</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・インポート</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>インポートクラス名</t>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>デフォルト値の変形</t>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -188,8 +292,27 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,8 +349,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -567,13 +696,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -649,10 +935,73 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="3" xr:uid="{5795358E-B3D9-E246-AA93-196E8A7B98B0}"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -729,8 +1078,26 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="valueObject"/>
+      <sheetName val="config"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1054,17 +1421,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
@@ -1075,7 +1442,7 @@
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1083,17 +1450,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1469,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1481,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1126,7 +1493,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1138,7 +1505,7 @@
       <c r="E8" s="11"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1152,7 +1519,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1166,237 +1533,238 @@
       <c r="G10" s="12"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="32" t="s">
+    <row r="11" spans="1:10" s="35" customFormat="1">
+      <c r="A11" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:10" s="35" customFormat="1">
+      <c r="A12" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:10" s="35" customFormat="1">
+      <c r="A13" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="36" t="s">
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="39"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="39"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="3" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" s="35" customFormat="1">
+      <c r="A20" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="57"/>
+    </row>
+    <row r="21" spans="1:10" s="35" customFormat="1">
+      <c r="A21" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="60"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+    </row>
+    <row r="22" spans="1:10" s="35" customFormat="1">
+      <c r="A22" s="62"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="66"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" s="35" customFormat="1">
+      <c r="A23" s="62"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="66"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" s="35" customFormat="1">
+      <c r="A24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="66"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" s="35" customFormat="1">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="42" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A27" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B27" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C27" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D27" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E27" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="41" t="s">
+      <c r="F27" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="41"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A26" s="19"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="15"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="23"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="21"/>
@@ -1405,10 +1773,10 @@
       <c r="F29" s="21"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
+      <c r="I29" s="29"/>
       <c r="J29" s="15"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
@@ -1420,7 +1788,7 @@
       <c r="I30" s="23"/>
       <c r="J30" s="15"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
@@ -1432,7 +1800,7 @@
       <c r="I31" s="23"/>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
@@ -1444,44 +1812,158 @@
       <c r="I32" s="23"/>
       <c r="J32" s="15"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="21"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
       <c r="I33" s="23"/>
       <c r="J33" s="15"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="28"/>
+    <row r="34" spans="1:10">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
       <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="15"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="19"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="15"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="15"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E50">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E59" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{D91A6F7B-4D29-2449-B2A6-B2DE56883681}">
+      <formula1>createToString</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C13" xr:uid="{B0E32580-3EF3-AE41-8E80-2DD2D7B8B160}">
+      <formula1>adjustDefaultValue</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
@@ -1490,4 +1972,98 @@
     <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F84EA6D-49E1-CD4B-9AB8-6AA12DE91E95}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="256" width="8.83203125" style="47" customWidth="1"/>
+    <col min="257" max="16384" width="10.83203125" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="19">
+      <c r="A1" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="46"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="J4" s="50"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="53"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7"/>
+  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Still buggy. just for recording.
</commit_message>
<xml_diff>
--- a/meta/objects/ApiDeleteTelegram.xlsx
+++ b/meta/objects/ApiDeleteTelegram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGenerator/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FDC53D-686A-1F4E-B675-F41759DF323A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF64D58D-D3EC-DD47-BEC3-9B1D71D7C954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3940" yWindow="2260" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,6 @@
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="accessScope">config!$B$4:$B$6</definedName>
     <definedName name="accessScope2">config!$B$4:$B$5</definedName>
@@ -151,18 +148,6 @@
     <t>総称型</t>
   </si>
   <si>
-    <t>blanco.rest.valueobject</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>blanco\rest\valueobject</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>\blanco\rest\valueobject</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>バリューオブジェクト定義書 設定シート</t>
     <rPh sb="14" eb="16">
       <t>セッテイ</t>
@@ -244,6 +229,18 @@
   </si>
   <si>
     <t>デフォルト値の変形</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>blanco\restgenerator\valueobject</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>blanco.restgenerator.valueobject</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>\blanco\restgenerator\valueobject</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -923,18 +920,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -997,6 +982,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1083,21 +1080,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="valueObject"/>
-      <sheetName val="config"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1427,8 +1409,8 @@
   </sheetPr>
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1487,7 +1469,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="11"/>
@@ -1499,7 +1481,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D8" s="40"/>
       <c r="E8" s="11"/>
@@ -1534,23 +1516,23 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:10" s="35" customFormat="1">
-      <c r="A11" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
+      <c r="A11" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="52"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:10" s="35" customFormat="1">
-      <c r="A12" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56" t="s">
-        <v>34</v>
+      <c r="A12" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52" t="s">
+        <v>31</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1558,12 +1540,12 @@
       <c r="G12"/>
     </row>
     <row r="13" spans="1:10" s="35" customFormat="1">
-      <c r="A13" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56" t="s">
-        <v>34</v>
+      <c r="A13" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52" t="s">
+        <v>31</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -1615,7 +1597,7 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
@@ -1627,7 +1609,7 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
@@ -1644,62 +1626,62 @@
     </row>
     <row r="20" spans="1:10" s="35" customFormat="1">
       <c r="A20" s="32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="33"/>
-      <c r="G20" s="57"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="1:10" s="35" customFormat="1">
-      <c r="A21" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="A21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
       <c r="F21" s="37"/>
-      <c r="G21" s="60"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
+      <c r="G21" s="56"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
     </row>
     <row r="22" spans="1:10" s="35" customFormat="1">
-      <c r="A22" s="62"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="66"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="62"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" s="35" customFormat="1">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="66"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="62"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" s="35" customFormat="1">
-      <c r="A24" s="69"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="66"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="62"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -1729,37 +1711,37 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="41"/>
+      <c r="G27" s="69"/>
       <c r="H27" s="16"/>
       <c r="I27" s="17"/>
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
       <c r="H28" s="18"/>
       <c r="I28" s="30"/>
       <c r="J28" s="15"/>
@@ -1987,78 +1969,78 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="11" max="256" width="8.83203125" style="47" customWidth="1"/>
-    <col min="257" max="16384" width="10.83203125" style="47"/>
+    <col min="1" max="3" width="8.83203125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="43" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="43" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="256" width="8.83203125" style="43" customWidth="1"/>
+    <col min="257" max="16384" width="10.83203125" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46" t="s">
+      <c r="F3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="46"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="B3" s="48" t="s">
+      <c r="H3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="J3" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="48" t="s">
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="J4" s="46"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="D5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="B4" s="49"/>
-      <c r="D4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="J4" s="50"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="52" t="s">
-        <v>32</v>
+      <c r="F5" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="48" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="53"/>
+      <c r="B6" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7"/>

</xml_diff>